<commit_message>
make it work for template 1.0
</commit_message>
<xml_diff>
--- a/src/main/resources/csv2templatePath.xlsx
+++ b/src/main/resources/csv2templatePath.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ycao77/bmir-radx/radx-rad-metadata-compiler/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3775A608-1F7E-A44F-AC92-611459C18535}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2E7CEA8-C865-194D-A719-71B856091614}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-8360" yWindow="-28300" windowWidth="43800" windowHeight="28300" xr2:uid="{297628F6-E04B-2149-A12F-46F8E7030659}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="66">
   <si>
     <t>RADx-rad Field Label</t>
   </si>
@@ -228,6 +228,12 @@
   </si>
   <si>
     <t>/Data File Identity/File Name</t>
+  </si>
+  <si>
+    <t>keywords</t>
+  </si>
+  <si>
+    <t>/Data File Subjects/Keyword</t>
   </si>
 </sst>
 </file>
@@ -649,10 +655,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C9FA6C8-3052-4F44-924C-F8A85A6A2B10}">
-  <dimension ref="A1:B37"/>
+  <dimension ref="A1:B38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -957,6 +963,14 @@
         <v>61</v>
       </c>
     </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>